<commit_message>
system tests approved by tl
</commit_message>
<xml_diff>
--- a/SimpCity US11 Test.Document (3 Pass 0 Fail).xlsx
+++ b/SimpCity US11 Test.Document (3 Pass 0 Fail).xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huiyi\Downloads\Year 3-Poly\Sem 3.2 DevOps\Tesr Documents\Sprint 4 V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clari\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B92D40-1809-4434-B1D3-34C7564E9FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323D9A1E-84C3-498F-BDBC-1ABE642E8B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US11 Sprint 4 " sheetId="22" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="60">
   <si>
     <t>Test Scenarios for SimpCity</t>
   </si>
@@ -1181,38 +1181,38 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2143,31 +2143,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB0EBBF-B789-4513-8DC1-DC35A3897BCA}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" customWidth="1"/>
-    <col min="4" max="4" width="71.42578125" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="8"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="58.33203125" customWidth="1"/>
+    <col min="4" max="4" width="71.44140625" customWidth="1"/>
+    <col min="5" max="5" width="44.5546875" customWidth="1"/>
+    <col min="6" max="6" width="31.109375" style="8" customWidth="1"/>
     <col min="7" max="7" width="18" style="66" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="8" customWidth="1"/>
     <col min="9" max="9" width="233" style="8" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="111"/>
+      <c r="C1" s="121"/>
       <c r="D1" s="37"/>
       <c r="E1" s="35"/>
       <c r="F1" s="39"/>
@@ -2178,29 +2178,29 @@
       <c r="K1" s="10"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
       <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="112"/>
+      <c r="C2" s="120"/>
       <c r="D2" s="13"/>
       <c r="E2" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="112"/>
+      <c r="F2" s="120"/>
       <c r="G2" s="78"/>
-      <c r="H2" s="112" t="s">
+      <c r="H2" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="112"/>
+      <c r="I2" s="120"/>
       <c r="J2" s="108" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="109"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="22" t="s">
         <v>5</v>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="44" t="s">
         <v>10</v>
@@ -2258,7 +2258,7 @@
       </c>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="23" t="s">
         <v>16</v>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="26" t="s">
         <v>17</v>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="110" t="s">
         <v>21</v>
@@ -2333,7 +2333,7 @@
       <c r="J7"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="57" t="s">
         <v>24</v>
@@ -2359,7 +2359,7 @@
       <c r="K8" s="33"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="45"/>
       <c r="C9" s="54"/>
@@ -2381,7 +2381,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="D10" s="5"/>
       <c r="E10" s="1"/>
@@ -2397,7 +2397,7 @@
       <c r="K10" s="9"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -2413,7 +2413,7 @@
       <c r="K11" s="11"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="67"/>
       <c r="B12" s="12"/>
       <c r="C12" s="51"/>
@@ -2426,7 +2426,7 @@
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
     </row>
-    <row r="13" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="68" t="s">
         <v>27</v>
       </c>
@@ -2461,31 +2461,31 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="65" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="113">
+    <row r="14" spans="1:12" s="65" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="111">
         <v>1</v>
       </c>
-      <c r="B14" s="115" t="s">
+      <c r="B14" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="117" t="s">
+      <c r="C14" s="115" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="119"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="121"/>
+      <c r="E14" s="117"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="119"/>
       <c r="I14" s="102"/>
       <c r="J14" s="77"/>
       <c r="K14" s="77"/>
     </row>
-    <row r="15" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="114"/>
-      <c r="B15" s="116"/>
-      <c r="C15" s="118"/>
+    <row r="15" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="112"/>
+      <c r="B15" s="114"/>
+      <c r="C15" s="116"/>
       <c r="D15" s="76" t="s">
         <v>47</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
       <c r="K15" s="97"/>
     </row>
-    <row r="16" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="87">
         <v>2</v>
       </c>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="K16" s="92"/>
     </row>
-    <row r="17" spans="1:11" s="75" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="75" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="86">
         <v>3</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="2"/>
       <c r="C18" s="72"/>
@@ -2580,7 +2580,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2593,7 +2593,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2606,7 +2606,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2619,28 +2619,28 @@
       <c r="J21" s="7"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="34"/>
       <c r="B22" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="112"/>
+      <c r="C22" s="120"/>
       <c r="D22" s="13"/>
       <c r="E22" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="112"/>
+      <c r="F22" s="120"/>
       <c r="G22" s="78"/>
-      <c r="H22" s="112" t="s">
+      <c r="H22" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="I22" s="112"/>
+      <c r="I22" s="120"/>
       <c r="J22" s="108" t="s">
         <v>4</v>
       </c>
       <c r="K22" s="109"/>
     </row>
-    <row r="23" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="22" t="s">
         <v>5</v>
@@ -2669,7 +2669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="44" t="s">
         <v>10</v>
@@ -2696,7 +2696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="17"/>
       <c r="B25" s="23" t="s">
         <v>16</v>
@@ -2723,7 +2723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
       <c r="B26" s="26" t="s">
         <v>17</v>
@@ -2750,7 +2750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="110" t="s">
         <v>21</v>
@@ -2768,7 +2768,7 @@
       <c r="I27" s="110"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="57" t="s">
         <v>24</v>
@@ -2791,7 +2791,7 @@
       <c r="J28" s="42"/>
       <c r="K28" s="33"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="45"/>
       <c r="C29" s="54"/>
@@ -2799,7 +2799,9 @@
       <c r="E29" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="58"/>
+      <c r="F29" s="58" t="s">
+        <v>15</v>
+      </c>
       <c r="G29" s="79"/>
       <c r="H29" s="62" t="s">
         <v>14</v>
@@ -2810,7 +2812,7 @@
       <c r="J29" s="21"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="D30" s="5"/>
       <c r="E30" s="1"/>
@@ -2825,7 +2827,7 @@
       <c r="J30" s="21"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -2840,7 +2842,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="67"/>
       <c r="B32" s="12"/>
       <c r="C32" s="51"/>
@@ -2853,7 +2855,7 @@
       <c r="J32" s="14"/>
       <c r="K32" s="15"/>
     </row>
-    <row r="33" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A33" s="68" t="s">
         <v>27</v>
       </c>
@@ -2888,31 +2890,31 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="113">
+    <row r="34" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="A34" s="111">
         <v>1</v>
       </c>
-      <c r="B34" s="115" t="s">
+      <c r="B34" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="117" t="s">
+      <c r="C34" s="115" t="s">
         <v>45</v>
       </c>
       <c r="D34" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="119"/>
-      <c r="F34" s="120"/>
-      <c r="G34" s="120"/>
-      <c r="H34" s="121"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="119"/>
       <c r="I34" s="102"/>
       <c r="J34" s="77"/>
       <c r="K34" s="77"/>
     </row>
-    <row r="35" spans="1:11" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="114"/>
-      <c r="B35" s="116"/>
-      <c r="C35" s="118"/>
+    <row r="35" spans="1:11" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="112"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="116"/>
       <c r="D35" s="76" t="s">
         <v>47</v>
       </c>
@@ -2934,7 +2936,7 @@
       </c>
       <c r="K35" s="97"/>
     </row>
-    <row r="36" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A36" s="87">
         <v>2</v>
       </c>
@@ -2963,7 +2965,7 @@
       </c>
       <c r="K36" s="92"/>
     </row>
-    <row r="37" spans="1:11" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="86">
         <v>3</v>
       </c>
@@ -2994,6 +2996,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="E27:F27"/>
@@ -3002,21 +3019,6 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="E34:H34"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 I5 F5 C25 I25 F25" xr:uid="{67241214-CE61-44FF-8B74-B06C36F5319C}">

</xml_diff>